<commit_message>
cleaning the notebooks a little
</commit_message>
<xml_diff>
--- a/results/city-frequencies.xlsx
+++ b/results/city-frequencies.xlsx
@@ -16,12 +16,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
   <si>
+    <t>Berlin</t>
+  </si>
+  <si>
     <t>Bochum</t>
   </si>
   <si>
-    <t>Berlin</t>
-  </si>
-  <si>
     <t>Dortmund</t>
   </si>
   <si>
@@ -31,24 +31,24 @@
     <t>Wien</t>
   </si>
   <si>
+    <t>Trier</t>
+  </si>
+  <si>
     <t>Marbach</t>
   </si>
   <si>
     <t>Halle-Wittenberg</t>
   </si>
   <si>
-    <t>Trier</t>
-  </si>
-  <si>
     <t>Gießen</t>
   </si>
   <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
     <t>Hannover</t>
   </si>
   <si>
-    <t>Hamburg</t>
-  </si>
-  <si>
     <t>Göttingen</t>
   </si>
   <si>
@@ -73,24 +73,24 @@
     <t>Salzburg</t>
   </si>
   <si>
+    <t>Potsdam</t>
+  </si>
+  <si>
     <t>Tübingen</t>
   </si>
   <si>
-    <t>Potsdam</t>
-  </si>
-  <si>
     <t>Bergen</t>
   </si>
   <si>
     <t>Duisburg</t>
   </si>
   <si>
+    <t>Wolfenbüttel</t>
+  </si>
+  <si>
     <t>Braunschweig</t>
   </si>
   <si>
-    <t>Wolfenbüttel</t>
-  </si>
-  <si>
     <t>Mannheim</t>
   </si>
   <si>
@@ -157,12 +157,12 @@
     <t>Wuppertal</t>
   </si>
   <si>
+    <t>Delft, Netherlands</t>
+  </si>
+  <si>
     <t>Luxembourg</t>
   </si>
   <si>
-    <t>Delft, Netherlands</t>
-  </si>
-  <si>
     <t>Kassel</t>
   </si>
   <si>
@@ -280,12 +280,12 @@
     <t>Verona</t>
   </si>
   <si>
+    <t>Kopenhagen</t>
+  </si>
+  <si>
     <t>Lissabon</t>
   </si>
   <si>
-    <t>Kopenhagen</t>
-  </si>
-  <si>
     <t>Bologna</t>
   </si>
   <si>
@@ -349,12 +349,12 @@
     <t>Luzern</t>
   </si>
   <si>
+    <t>London</t>
+  </si>
+  <si>
     <t>Athens</t>
   </si>
   <si>
-    <t>London</t>
-  </si>
-  <si>
     <t>Budapest</t>
   </si>
   <si>
@@ -382,10 +382,10 @@
     <t>Santa Barbara</t>
   </si>
   <si>
+    <t>Cork</t>
+  </si>
+  <si>
     <t>Glasgow</t>
-  </si>
-  <si>
-    <t>Cork</t>
   </si>
   <si>
     <t>Frankfurt am Main</t>
@@ -1179,10 +1179,10 @@
         <v>128</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C2">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1194,22 +1194,22 @@
         <v>4</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2">
         <v>7</v>
       </c>
-      <c r="J2">
-        <v>3</v>
-      </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
       <c r="L2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="M2">
         <v>5</v>
@@ -1236,10 +1236,10 @@
         <v>2</v>
       </c>
       <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
         <v>5</v>
-      </c>
-      <c r="V2">
-        <v>1</v>
       </c>
       <c r="W2">
         <v>2</v>
@@ -1565,10 +1565,10 @@
         <v>129</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C3">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1580,22 +1580,22 @@
         <v>13</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M3">
         <v>6</v>
@@ -1634,10 +1634,10 @@
         <v>0</v>
       </c>
       <c r="Y3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Z3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AA3">
         <v>0</v>
@@ -1951,10 +1951,10 @@
         <v>130</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C4">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1966,22 +1966,22 @@
         <v>11</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J4">
         <v>3</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="L4">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M4">
         <v>13</v>
@@ -2020,10 +2020,10 @@
         <v>1</v>
       </c>
       <c r="Y4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Z4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AA4">
         <v>4</v>
@@ -2092,10 +2092,10 @@
         <v>0</v>
       </c>
       <c r="AW4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY4">
         <v>1</v>
@@ -2337,10 +2337,10 @@
         <v>131</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2352,10 +2352,10 @@
         <v>9</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -2364,10 +2364,10 @@
         <v>2</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M5">
         <v>9</v>
@@ -2394,10 +2394,10 @@
         <v>1</v>
       </c>
       <c r="U5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="V5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="W5">
         <v>0</v>
@@ -2406,10 +2406,10 @@
         <v>0</v>
       </c>
       <c r="Y5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AA5">
         <v>2</v>
@@ -2723,10 +2723,10 @@
         <v>132</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C6">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -2738,22 +2738,22 @@
         <v>15</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
         <v>4</v>
       </c>
-      <c r="I6">
-        <v>5</v>
-      </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L6">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="M6">
         <v>9</v>
@@ -2780,10 +2780,10 @@
         <v>0</v>
       </c>
       <c r="U6">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="V6">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="W6">
         <v>0</v>
@@ -2792,10 +2792,10 @@
         <v>0</v>
       </c>
       <c r="Y6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AA6">
         <v>2</v>
@@ -2864,10 +2864,10 @@
         <v>3</v>
       </c>
       <c r="AW6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY6">
         <v>1</v>
@@ -3109,10 +3109,10 @@
         <v>133</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C7">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -3127,19 +3127,19 @@
         <v>0</v>
       </c>
       <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
         <v>4</v>
       </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="M7">
         <v>8</v>
@@ -3166,10 +3166,10 @@
         <v>0</v>
       </c>
       <c r="U7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W7">
         <v>0</v>
@@ -3178,10 +3178,10 @@
         <v>0</v>
       </c>
       <c r="Y7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Z7">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AA7">
         <v>3</v>
@@ -3250,10 +3250,10 @@
         <v>1</v>
       </c>
       <c r="AW7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY7">
         <v>0</v>
@@ -3495,10 +3495,10 @@
         <v>134</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -3510,22 +3510,22 @@
         <v>9</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="L8">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="M8">
         <v>1</v>
@@ -3552,10 +3552,10 @@
         <v>1</v>
       </c>
       <c r="U8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="V8">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="W8">
         <v>1</v>
@@ -3564,10 +3564,10 @@
         <v>1</v>
       </c>
       <c r="Y8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AA8">
         <v>2</v>
@@ -3881,10 +3881,10 @@
         <v>135</v>
       </c>
       <c r="B9">
+        <v>32</v>
+      </c>
+      <c r="C9">
         <v>4</v>
-      </c>
-      <c r="C9">
-        <v>32</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -3896,22 +3896,22 @@
         <v>11</v>
       </c>
       <c r="G9">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
         <v>4</v>
       </c>
-      <c r="I9">
-        <v>8</v>
-      </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M9">
         <v>7</v>
@@ -3938,10 +3938,10 @@
         <v>0</v>
       </c>
       <c r="U9">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="V9">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="W9">
         <v>0</v>
@@ -3950,10 +3950,10 @@
         <v>0</v>
       </c>
       <c r="Y9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Z9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA9">
         <v>2</v>
@@ -4022,10 +4022,10 @@
         <v>2</v>
       </c>
       <c r="AW9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AX9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AY9">
         <v>0</v>
@@ -4145,10 +4145,10 @@
         <v>0</v>
       </c>
       <c r="CL9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CM9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CN9">
         <v>0</v>
@@ -4267,10 +4267,10 @@
         <v>136</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="C10">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -4282,22 +4282,22 @@
         <v>6</v>
       </c>
       <c r="G10">
+        <v>12</v>
+      </c>
+      <c r="H10">
         <v>4</v>
       </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
       <c r="I10">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="L10">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M10">
         <v>12</v>
@@ -4324,10 +4324,10 @@
         <v>0</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="V10">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="W10">
         <v>0</v>
@@ -4336,10 +4336,10 @@
         <v>2</v>
       </c>
       <c r="Y10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Z10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AA10">
         <v>4</v>
@@ -4408,10 +4408,10 @@
         <v>3</v>
       </c>
       <c r="AW10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY10">
         <v>0</v>

</xml_diff>